<commit_message>
flatten half working, same with tostring
</commit_message>
<xml_diff>
--- a/pseudo/truth table.xlsx
+++ b/pseudo/truth table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\rust\math-eval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\rust\math-eval\pseudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5249AE1E-1E76-4513-942D-985F4CFB8D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77EEDCA-6768-4DAC-B3B1-0DC9DA3B115B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="21705" activeTab="1" xr2:uid="{D11C0042-871A-40E6-9C8F-06A0F0CE9C5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" activeTab="2" xr2:uid="{D11C0042-871A-40E6-9C8F-06A0F0CE9C5E}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED328C6-EFE2-46B0-B3DC-077C3296D415}">
   <dimension ref="E6:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="G4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E981DE-46EA-495E-91FA-884FEE494070}">
   <dimension ref="E8"/>
   <sheetViews>
-    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>